<commit_message>
feat: funciona con la primera matrícula, espera fija
</commit_message>
<xml_diff>
--- a/archivos/prueba1_modelos.xlsx
+++ b/archivos/prueba1_modelos.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AUTODOC España - tienda online de recambios coche con más de 4 millones de repuestos coches</t>
+          <t>Audi A4 B6 1.9 TDI 130 cv Gasóleo 2000 - 2004 AVF, AWX</t>
         </is>
       </c>
     </row>
@@ -465,7 +465,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AUTODOC España - tienda online de recambios coche con más de 4 millones de repuestos coches</t>
+          <t xml:space="preserve">Error: Message: stale element reference: stale element not found
+  (Session info: chrome=130.0.6723.70); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#stale-element-reference-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF616893AB5+28005]
+	(No symbol) [0x00007FF6167F83B0]
+	(No symbol) [0x00007FF61669580A]
+	(No symbol) [0x00007FF6166A7D0B]
+	(No symbol) [0x00007FF61669CF04]
+	(No symbol) [0x00007FF61669AE09]
+	(No symbol) [0x00007FF61669E5E7]
+	(No symbol) [0x00007FF61669E6A0]
+	(No symbol) [0x00007FF6166E7B4B]
+	(No symbol) [0x00007FF6166DB3AC]
+	(No symbol) [0x00007FF61670BA3A]
+	(No symbol) [0x00007FF6166D9246]
+	(No symbol) [0x00007FF61670BC50]
+	(No symbol) [0x00007FF61672B8B3]
+	(No symbol) [0x00007FF61670B7E3]
+	(No symbol) [0x00007FF6166D75C8]
+	(No symbol) [0x00007FF6166D8731]
+	GetHandleVerifier [0x00007FF616B8643D+3118829]
+	GetHandleVerifier [0x00007FF616BD6C90+3448640]
+	GetHandleVerifier [0x00007FF616BCCF0D+3408317]
+	GetHandleVerifier [0x00007FF61695A40B+841403]
+	(No symbol) [0x00007FF61680340F]
+	(No symbol) [0x00007FF6167FF484]
+	(No symbol) [0x00007FF6167FF61D]
+	(No symbol) [0x00007FF6167EEB79]
+	BaseThreadInitThunk [0x00007FFB490D7374+20]
+	RtlUserThreadStart [0x00007FFB4A61CC91+33]
+</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: iniciar y cerrar driver por cada oferta, para tener control de los que no encuentre resultados
</commit_message>
<xml_diff>
--- a/archivos/prueba1_modelos.xlsx
+++ b/archivos/prueba1_modelos.xlsx
@@ -463,41 +463,7 @@
           <t>3206fvm</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Error: Message: stale element reference: stale element not found
-  (Session info: chrome=130.0.6723.70); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#stale-element-reference-exception
-Stacktrace:
-	GetHandleVerifier [0x00007FF616893AB5+28005]
-	(No symbol) [0x00007FF6167F83B0]
-	(No symbol) [0x00007FF61669580A]
-	(No symbol) [0x00007FF6166A7D0B]
-	(No symbol) [0x00007FF61669CF04]
-	(No symbol) [0x00007FF61669AE09]
-	(No symbol) [0x00007FF61669E5E7]
-	(No symbol) [0x00007FF61669E6A0]
-	(No symbol) [0x00007FF6166E7B4B]
-	(No symbol) [0x00007FF6166DB3AC]
-	(No symbol) [0x00007FF61670BA3A]
-	(No symbol) [0x00007FF6166D9246]
-	(No symbol) [0x00007FF61670BC50]
-	(No symbol) [0x00007FF61672B8B3]
-	(No symbol) [0x00007FF61670B7E3]
-	(No symbol) [0x00007FF6166D75C8]
-	(No symbol) [0x00007FF6166D8731]
-	GetHandleVerifier [0x00007FF616B8643D+3118829]
-	GetHandleVerifier [0x00007FF616BD6C90+3448640]
-	GetHandleVerifier [0x00007FF616BCCF0D+3408317]
-	GetHandleVerifier [0x00007FF61695A40B+841403]
-	(No symbol) [0x00007FF61680340F]
-	(No symbol) [0x00007FF6167FF484]
-	(No symbol) [0x00007FF6167FF61D]
-	(No symbol) [0x00007FF6167EEB79]
-	BaseThreadInitThunk [0x00007FFB490D7374+20]
-	RtlUserThreadStart [0x00007FFB4A61CC91+33]
-</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>